<commit_message>
[M]Update test scenario for test case Warranty_0005
</commit_message>
<xml_diff>
--- a/Barco_Interview_Assignment.xlsx
+++ b/Barco_Interview_Assignment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eric\work_space\面試\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eric\work_space\python_project\interview_projects\barco_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C974D-6101-40B6-87D0-26F315481476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC985146-FF56-429B-AAD7-74230BD4AFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B981A212-49AE-4D75-82AE-7DC0C09D4913}"/>
   </bookViews>
@@ -212,10 +212,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Get warranty info with number length = 1/4/5/6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">1. The device info is correct
 2. The info format as below:
 </t>
@@ -279,6 +275,10 @@
     <t>Step1: https://www.barco.com/eu-en/support/clickshare-extended-warranty/warranty
 Step2: input 1/1111/11111/111111 in the SN field
 Step3: Clicks on "Get Info" Button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get warranty info with number length = 1/4/5/6/10/11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -398,17 +398,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B91828-2F4B-42EA-8CAF-CBF464E12D70}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:H9"/>
     </sheetView>
   </sheetViews>
@@ -949,237 +949,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="C4:H5"/>
+    <mergeCell ref="C8:H9"/>
+    <mergeCell ref="C10:H11"/>
     <mergeCell ref="C12:H13"/>
     <mergeCell ref="C16:H17"/>
     <mergeCell ref="C18:H19"/>
@@ -1190,15 +1199,6 @@
     <mergeCell ref="A18:B19"/>
     <mergeCell ref="C14:H15"/>
     <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="C4:H5"/>
-    <mergeCell ref="C8:H9"/>
-    <mergeCell ref="C10:H11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA101BA-67B4-4336-A6FC-4C2B091644B9}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="2" spans="1:7" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="3" spans="1:7" ht="178.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -1285,12 +1285,12 @@
         <v>21</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="5" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1324,13 +1324,13 @@
     </row>
     <row r="6" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="7" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="8" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -1395,7 +1395,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>